<commit_message>
here ya go, update on the work metrics
</commit_message>
<xml_diff>
--- a/documentation/WorkMetric.xlsx
+++ b/documentation/WorkMetric.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="37">
   <si>
     <t>Chris Lockhart</t>
   </si>
@@ -116,6 +116,18 @@
   <si>
     <t>December</t>
   </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sept</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
 </sst>
 </file>
 
@@ -415,7 +427,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="135" wrapText="1"/>
@@ -466,6 +478,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -486,7 +499,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -548,6 +561,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -610,6 +624,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -672,6 +687,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -734,23 +750,24 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="101421440"/>
-        <c:axId val="101422976"/>
+        <c:axId val="97889280"/>
+        <c:axId val="97899264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101421440"/>
+        <c:axId val="97889280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101422976"/>
+        <c:crossAx val="97899264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101422976"/>
+        <c:axId val="97899264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +775,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101421440"/>
+        <c:crossAx val="97889280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -771,7 +788,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -854,7 +871,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -928,7 +945,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1002,7 +1019,372 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$75</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Engine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$H$74</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sept</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$75:$H$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$76</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Game</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$H$74</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sept</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$76:$H$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GUI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$H$74</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sept</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$77:$H$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Networking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$H$74</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sept</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$78:$H$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$79</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Input</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$H$74</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sept</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$79:$H$79</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="101531008"/>
+        <c:axId val="101529472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="101531008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101529472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="101529472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101531008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1125,6 +1507,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1418,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:V67"/>
+  <dimension ref="C4:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3703,6 +4115,152 @@
       <c r="H67" s="20">
         <f>SUM(D46,K46,R46)</f>
         <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" ht="15.75" thickBot="1"/>
+    <row r="74" spans="3:8">
+      <c r="C74" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H74" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8">
+      <c r="C75" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="16">
+        <f>O9</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="16">
+        <f>O17</f>
+        <v>73.599999999999994</v>
+      </c>
+      <c r="F75" s="16">
+        <f>O25</f>
+        <v>53.6</v>
+      </c>
+      <c r="G75" s="16">
+        <f>O33</f>
+        <v>50</v>
+      </c>
+      <c r="H75" s="17">
+        <f>O41</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8">
+      <c r="C76" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="16">
+        <f t="shared" ref="D76:D79" si="18">O10</f>
+        <v>0</v>
+      </c>
+      <c r="E76" s="16">
+        <f t="shared" ref="E76:E79" si="19">O18</f>
+        <v>0</v>
+      </c>
+      <c r="F76" s="16">
+        <f t="shared" ref="F76:F79" si="20">O26</f>
+        <v>31</v>
+      </c>
+      <c r="G76" s="16">
+        <f t="shared" ref="G76:G79" si="21">O34</f>
+        <v>35</v>
+      </c>
+      <c r="H76" s="17">
+        <f t="shared" ref="H76:H79" si="22">O42</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8">
+      <c r="C77" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="16">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E77" s="16">
+        <f t="shared" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="F77" s="16">
+        <f t="shared" si="20"/>
+        <v>59</v>
+      </c>
+      <c r="G77" s="16">
+        <f t="shared" si="21"/>
+        <v>15</v>
+      </c>
+      <c r="H77" s="17">
+        <f t="shared" si="22"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8">
+      <c r="C78" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="16">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="16">
+        <f t="shared" si="19"/>
+        <v>50</v>
+      </c>
+      <c r="F78" s="16">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G78" s="16">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H78" s="17">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" ht="15.75" thickBot="1">
+      <c r="C79" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="19">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E79" s="19">
+        <f t="shared" si="19"/>
+        <v>20</v>
+      </c>
+      <c r="F79" s="19">
+        <f t="shared" si="20"/>
+        <v>50</v>
+      </c>
+      <c r="G79" s="19">
+        <f t="shared" si="21"/>
+        <v>15</v>
+      </c>
+      <c r="H79" s="20">
+        <f t="shared" si="22"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>